<commit_message>
Reorganizado el archivo de Excel
Para mejor lectura
</commit_message>
<xml_diff>
--- a/Documentos/Sprints.xlsx
+++ b/Documentos/Sprints.xlsx
@@ -1117,9 +1117,6 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color rgb="FF808080"/>
@@ -1220,6 +1217,9 @@
           <color rgb="FF000000"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
@@ -1625,7 +1625,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sprint 1 - Grupo'!$K$4</c:f>
+              <c:f>'Sprint 1 - Grupo'!$Q$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1713,7 +1713,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Sprint 1 - Grupo'!$L$3:$P$3</c:f>
+              <c:f>'Sprint 1 - Grupo'!$R$3:$V$3</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -1736,7 +1736,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 1 - Grupo'!$L$4:$P$4</c:f>
+              <c:f>'Sprint 1 - Grupo'!$R$4:$V$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1770,7 +1770,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sprint 1 - Grupo'!$K$5</c:f>
+              <c:f>'Sprint 1 - Grupo'!$Q$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1858,7 +1858,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Sprint 1 - Grupo'!$L$3:$P$3</c:f>
+              <c:f>'Sprint 1 - Grupo'!$R$3:$V$3</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -1881,7 +1881,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 1 - Grupo'!$L$5:$P$5</c:f>
+              <c:f>'Sprint 1 - Grupo'!$R$5:$V$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2195,7 +2195,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sprint 1 - Grupo'!$K$15</c:f>
+              <c:f>'Sprint 1 - Grupo'!$Q$15</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2283,7 +2283,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Sprint 1 - Grupo'!$L$14:$P$14</c:f>
+              <c:f>'Sprint 1 - Grupo'!$R$14:$V$14</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -2306,7 +2306,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 1 - Grupo'!$L$15:$P$15</c:f>
+              <c:f>'Sprint 1 - Grupo'!$R$15:$V$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2340,7 +2340,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sprint 1 - Grupo'!$K$16</c:f>
+              <c:f>'Sprint 1 - Grupo'!$Q$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2428,7 +2428,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Sprint 1 - Grupo'!$L$14:$P$14</c:f>
+              <c:f>'Sprint 1 - Grupo'!$R$14:$V$14</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -2451,7 +2451,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 1 - Grupo'!$L$16:$P$16</c:f>
+              <c:f>'Sprint 1 - Grupo'!$R$16:$V$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2765,7 +2765,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sprint 1 - Grupo'!$K$27</c:f>
+              <c:f>'Sprint 1 - Grupo'!$Q$27</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2853,7 +2853,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Sprint 1 - Grupo'!$L$26:$P$26</c:f>
+              <c:f>'Sprint 1 - Grupo'!$R$26:$V$26</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -2876,7 +2876,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 1 - Grupo'!$L$27:$P$27</c:f>
+              <c:f>'Sprint 1 - Grupo'!$R$27:$V$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2910,7 +2910,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sprint 1 - Grupo'!$K$28</c:f>
+              <c:f>'Sprint 1 - Grupo'!$Q$28</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2998,7 +2998,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Sprint 1 - Grupo'!$L$26:$P$26</c:f>
+              <c:f>'Sprint 1 - Grupo'!$R$26:$V$26</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -3021,7 +3021,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 1 - Grupo'!$L$28:$P$28</c:f>
+              <c:f>'Sprint 1 - Grupo'!$R$28:$V$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -3335,7 +3335,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sprint 1 - Grupo'!$K$38</c:f>
+              <c:f>'Sprint 1 - Grupo'!$Q$38</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3423,7 +3423,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Sprint 1 - Grupo'!$L$37:$P$37</c:f>
+              <c:f>'Sprint 1 - Grupo'!$R$37:$V$37</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -3446,7 +3446,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 1 - Grupo'!$L$38:$P$38</c:f>
+              <c:f>'Sprint 1 - Grupo'!$R$38:$V$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -3480,7 +3480,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sprint 1 - Grupo'!$K$39</c:f>
+              <c:f>'Sprint 1 - Grupo'!$Q$39</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3568,7 +3568,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Sprint 1 - Grupo'!$L$37:$P$37</c:f>
+              <c:f>'Sprint 1 - Grupo'!$R$37:$V$37</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -3591,7 +3591,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 1 - Grupo'!$L$39:$P$39</c:f>
+              <c:f>'Sprint 1 - Grupo'!$R$39:$V$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -3905,7 +3905,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sprint 1 - Grupo'!$K$49</c:f>
+              <c:f>'Sprint 1 - Grupo'!$Q$49</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3993,7 +3993,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Sprint 1 - Grupo'!$L$48:$P$48</c:f>
+              <c:f>'Sprint 1 - Grupo'!$R$48:$V$48</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -4016,7 +4016,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 1 - Grupo'!$L$49:$P$49</c:f>
+              <c:f>'Sprint 1 - Grupo'!$R$49:$V$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -4050,7 +4050,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sprint 1 - Grupo'!$K$50</c:f>
+              <c:f>'Sprint 1 - Grupo'!$Q$50</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4138,7 +4138,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Sprint 1 - Grupo'!$L$48:$P$48</c:f>
+              <c:f>'Sprint 1 - Grupo'!$R$48:$V$48</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -4161,7 +4161,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 1 - Grupo'!$L$50:$P$50</c:f>
+              <c:f>'Sprint 1 - Grupo'!$R$50:$V$50</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -4415,19 +4415,12 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="lt1">
-                    <a:lumMod val="95000"/>
+                    <a:lumMod val="85000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:effectLst>
-                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-                    <a:prstClr val="black">
-                      <a:alpha val="40000"/>
-                    </a:prstClr>
-                  </a:outerShdw>
-                </a:effectLst>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
@@ -4454,19 +4447,12 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="lt1">
-                  <a:lumMod val="95000"/>
+                  <a:lumMod val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:effectLst>
-                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-                  <a:prstClr val="black">
-                    <a:alpha val="40000"/>
-                  </a:prstClr>
-                </a:outerShdw>
-              </a:effectLst>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
@@ -4487,7 +4473,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sprint 1 - Grupo'!$A$64</c:f>
+              <c:f>'Sprint 1 - Grupo'!$Q$54</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4497,26 +4483,82 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="34925" cap="rnd">
+            <a:ln w="22225" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
-              <a:round/>
             </a:ln>
             <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
             </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="es-ES"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Sprint 1 - Grupo'!$B$63:$F$63</c:f>
+              <c:f>'Sprint 1 - Grupo'!$R$53:$V$53</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -4539,7 +4581,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 1 - Grupo'!$B$64:$F$64</c:f>
+              <c:f>'Sprint 1 - Grupo'!$R$54:$V$54</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -4573,7 +4615,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sprint 1 - Grupo'!$A$65</c:f>
+              <c:f>'Sprint 1 - Grupo'!$Q$55</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4583,26 +4625,82 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="34925" cap="rnd">
+            <a:ln w="22225" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
-              <a:round/>
             </a:ln>
             <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent2">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
             </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="es-ES"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Sprint 1 - Grupo'!$B$63:$F$63</c:f>
+              <c:f>'Sprint 1 - Grupo'!$R$53:$V$53</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -4625,7 +4723,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 1 - Grupo'!$B$65:$F$65</c:f>
+              <c:f>'Sprint 1 - Grupo'!$R$55:$V$55</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -4655,8 +4753,9 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="ctr"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -4673,20 +4772,39 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="0">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="lt1">
-                <a:lumMod val="95000"/>
-                <a:alpha val="10000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
+          <a:ln>
+            <a:noFill/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -4698,7 +4816,7 @@
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="lt1">
-                    <a:lumMod val="85000"/>
+                    <a:lumMod val="75000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -4726,12 +4844,23 @@
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="95000"/>
-                  <a:alpha val="10000"/>
-                </a:schemeClr>
-              </a:solidFill>
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="0">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -4756,7 +4885,7 @@
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="lt1">
-                    <a:lumMod val="85000"/>
+                    <a:lumMod val="75000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -4780,7 +4909,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="t"/>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -4798,7 +4927,7 @@
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="lt1">
-                  <a:lumMod val="85000"/>
+                  <a:lumMod val="75000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -4815,28 +4944,20 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:gradFill flip="none" rotWithShape="1">
-      <a:gsLst>
-        <a:gs pos="0">
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:gs>
-        <a:gs pos="100000">
-          <a:schemeClr val="dk1">
-            <a:lumMod val="85000"/>
-            <a:lumOff val="15000"/>
-          </a:schemeClr>
-        </a:gs>
-      </a:gsLst>
-      <a:path path="circle">
-        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-      </a:path>
-      <a:tileRect/>
-    </a:gradFill>
-    <a:ln>
-      <a:noFill/>
+    <a:solidFill>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
     </a:ln>
     <a:effectLst/>
   </c:spPr>
@@ -7939,17 +8060,17 @@
 </file>
 
 <file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="236">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
@@ -7957,52 +8078,36 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="10000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:gradFill flip="none" rotWithShape="1">
-        <a:gsLst>
-          <a:gs pos="0">
-            <a:schemeClr val="dk1">
-              <a:lumMod val="65000"/>
-              <a:lumOff val="35000"/>
-            </a:schemeClr>
-          </a:gs>
-          <a:gs pos="100000">
-            <a:schemeClr val="dk1">
-              <a:lumMod val="85000"/>
-              <a:lumOff val="15000"/>
-            </a:schemeClr>
-          </a:gs>
-        </a:gsLst>
-        <a:path path="circle">
-          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-        </a:path>
-        <a:tileRect/>
-      </a:gradFill>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -8010,7 +8115,7 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -8020,14 +8125,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="15000"/>
+        <a:lumOff val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="lt1"/>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
       </a:solidFill>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -8036,72 +8144,131 @@
     </cs:bodyPr>
   </cs:dataLabelCallout>
   <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
+    <cs:effectRef idx="0">
       <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="34925" cap="rnd">
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:round/>
       </a:ln>
+      <a:effectLst>
+        <a:glow rad="139700">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="14000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
     </cs:spPr>
   </cs:dataPointLine>
   <cs:dataPointMarker>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="3">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+          <a:lumOff val="40000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -8118,15 +8285,15 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -8138,211 +8305,222 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:prstDash val="dash"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="10000"/>
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="5000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:prstDash val="dash"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+                <a:alpha val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+                <a:alpha val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
   </cs:seriesLine>
   <cs:title>
     <cs:lnRef idx="0"/>
@@ -8350,18 +8528,10 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="lt1">
-        <a:lumMod val="95000"/>
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
-      <a:effectLst>
-        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-          <a:prstClr val="black">
-            <a:alpha val="40000"/>
-          </a:prstClr>
-        </a:outerShdw>
-      </a:effectLst>
-    </cs:defRPr>
+    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -8370,12 +8540,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="rnd">
         <a:solidFill>
-          <a:schemeClr val="phClr"/>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
         </a:solidFill>
       </a:ln>
     </cs:spPr>
@@ -8386,7 +8558,7 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -8396,19 +8568,21 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="lt1"/>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -8418,7 +8592,7 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -8428,7 +8602,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
@@ -8438,16 +8612,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>239569</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>499343</xdr:colOff>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>172607</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>461818</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>173183</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1622137</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8468,16 +8642,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>239568</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>172605</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>291522</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>16742</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>447387</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>57727</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>329045</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>17318</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8498,16 +8672,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>239569</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>18761</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>516661</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>70715</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>418523</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>129886</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1596160</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>164522</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8528,16 +8702,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>239569</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>158173</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>308842</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>88899</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>389659</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>14432</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>329046</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>138545</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8558,15 +8732,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>225137</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>177513</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1506683</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>4331</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>404091</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>525319</xdr:colOff>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>173182</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -8588,16 +8762,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>239567</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>89889</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>54428</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>635001</xdr:colOff>
-      <xdr:row>73</xdr:row>
-      <xdr:rowOff>14432</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>1088571</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>32987</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8642,60 +8816,71 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabla6" displayName="Tabla6" ref="K48:P50" totalsRowShown="0">
-  <autoFilter ref="K48:P50"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="Q14:V16" totalsRowShown="0">
+  <autoFilter ref="Q14:V16"/>
   <tableColumns count="6">
     <tableColumn id="6" name="Tipo"/>
     <tableColumn id="1" name="Horas Iniciales">
-      <calculatedColumnFormula>Tabla182023[[#This Row],[Horas Totales 
-Asignadas por Tarea]]+C50+C51+C52+C53+C54+C55+C56</calculatedColumnFormula>
+      <calculatedColumnFormula>Tabla1820[[#This Row],[Horas Totales 
+Asignadas por Tarea]]+C23+C16+C17+C18+C19+C20+C21+C22</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" name="Semana 1">
-      <calculatedColumnFormula>L49-Tabla182023[[#This Row],[Primera Semana]]-D50</calculatedColumnFormula>
+      <calculatedColumnFormula>R15--Tabla1820[[#This Row],[Primera Semana]]-D16-D17</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" name="Semana 2">
-      <calculatedColumnFormula>M49-E51-E52</calculatedColumnFormula>
+      <calculatedColumnFormula>S15-E18-E19</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" name="Semana 3">
-      <calculatedColumnFormula>N49-F53-F54</calculatedColumnFormula>
+      <calculatedColumnFormula>T15-F21-F20</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" name="Semana 4">
-      <calculatedColumnFormula>O49-G55-G56</calculatedColumnFormula>
+      <calculatedColumnFormula>U15-G23-G22</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Tabla612" displayName="Tabla612" ref="A63:F65" totalsRowShown="0">
-  <autoFilter ref="A63:F65"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="Q3:V5" totalsRowShown="0">
+  <autoFilter ref="Q3:V5"/>
   <tableColumns count="6">
-    <tableColumn id="6" name="Tipo"/>
-    <tableColumn id="1" name="Horas Iniciales"/>
-    <tableColumn id="2" name="Semana 1"/>
-    <tableColumn id="3" name="Semana 2"/>
-    <tableColumn id="4" name="Semana 3"/>
-    <tableColumn id="5" name="Semana 4"/>
+    <tableColumn id="7" name="Tipo"/>
+    <tableColumn id="1" name="Horas Iniciales" dataDxfId="13">
+      <calculatedColumnFormula>Tabla18[[#This Row],[Horas Totales 
+Asignadas por Tarea]]+C5+C6+C7+C8+C9+C10+C11</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" name="Semana 1">
+      <calculatedColumnFormula>R4-Tabla18[[#This Row],[Primera Semana]]-D5</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" name="Semana 2">
+      <calculatedColumnFormula>S4-E6-E7</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" name="Semana 3">
+      <calculatedColumnFormula>T4-F8-F9</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" name="Semana 4">
+      <calculatedColumnFormula>U4-G10-G11</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
-  <tableStyleInfo name="TableStyleDark4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tabla10" displayName="Tabla10" ref="A1:C8" totalsRowShown="0" tableBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tabla10" displayName="Tabla10" ref="A1:C8" totalsRowShown="0" tableBorderDxfId="12">
   <autoFilter ref="A1:C8"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Elemento"/>
-    <tableColumn id="5" name="Reunión Con Cuarto Año" dataDxfId="12"/>
-    <tableColumn id="2" name="Reunión Segundo Año" dataDxfId="11"/>
+    <tableColumn id="5" name="Reunión Con Cuarto Año" dataDxfId="11"/>
+    <tableColumn id="2" name="Reunión Segundo Año" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Tabla1015" displayName="Tabla1015" ref="A10:C17" totalsRowShown="0" tableBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Tabla1015" displayName="Tabla1015" ref="A10:C17" totalsRowShown="0" tableBorderDxfId="9">
   <autoFilter ref="A10:C17"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Elemento"/>
@@ -8707,7 +8892,7 @@
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Tabla1016" displayName="Tabla1016" ref="A19:C26" totalsRowShown="0" tableBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Tabla1016" displayName="Tabla1016" ref="A19:C26" totalsRowShown="0" tableBorderDxfId="8">
   <autoFilter ref="A19:C26"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Elemento"/>
@@ -8719,7 +8904,7 @@
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Tabla1017" displayName="Tabla1017" ref="A28:C35" totalsRowShown="0" tableBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Tabla1017" displayName="Tabla1017" ref="A28:C35" totalsRowShown="0" tableBorderDxfId="7">
   <autoFilter ref="A28:C35"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Elemento"/>
@@ -8736,11 +8921,11 @@
   <tableColumns count="8">
     <tableColumn id="10" name="Semana" dataCellStyle="Note"/>
     <tableColumn id="1" name="Trabajos_x000a_Designados" dataCellStyle="Note"/>
-    <tableColumn id="2" name="Horas Totales_x000a_Asignadas por Tarea" dataDxfId="7" dataCellStyle="20% - Énfasis1"/>
+    <tableColumn id="2" name="Horas Totales_x000a_Asignadas por Tarea" dataDxfId="6" dataCellStyle="20% - Énfasis1"/>
     <tableColumn id="3" name="Horas Trabajadas en Reunion" dataCellStyle="Entrada"/>
-    <tableColumn id="4" name="Horas Autónomas" dataDxfId="6" dataCellStyle="60% - Énfasis6"/>
+    <tableColumn id="4" name="Horas Autónomas" dataDxfId="5" dataCellStyle="60% - Énfasis6"/>
     <tableColumn id="5" name="Justifique las horas autónomas" dataCellStyle="Note"/>
-    <tableColumn id="6" name="Horas Totales" dataDxfId="5" dataCellStyle="Error">
+    <tableColumn id="6" name="Horas Totales" dataDxfId="4" dataCellStyle="Error">
       <calculatedColumnFormula>Tabla248918[[#This Row],[Horas Trabajadas en Reunion]]+Tabla248918[[#This Row],[Horas Autónomas]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" name="¿Completó el_x000a_Objetivo?" dataCellStyle="Note"/>
@@ -8759,7 +8944,7 @@
     <tableColumn id="3" name="Horas Trabajadas en Reunion" dataCellStyle="Entrada"/>
     <tableColumn id="4" name="Horas Autónomas" dataCellStyle="60% - Énfasis6"/>
     <tableColumn id="5" name="Justifique las horas autónomas" dataCellStyle="Note"/>
-    <tableColumn id="6" name="Horas Totales" dataDxfId="4" dataCellStyle="Error">
+    <tableColumn id="6" name="Horas Totales" dataDxfId="3" dataCellStyle="Error">
       <calculatedColumnFormula>Tabla24[[#This Row],[Horas Trabajadas en Reunion]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" name="¿Completó el_x000a_Objetivo?" dataCellStyle="Note"/>
@@ -8778,7 +8963,7 @@
     <tableColumn id="3" name="Horas Trabajadas en Reunion" dataCellStyle="Entrada"/>
     <tableColumn id="4" name="Horas Autónomas" dataCellStyle="60% - Énfasis6"/>
     <tableColumn id="5" name="Justifique las horas autónomas" dataCellStyle="Note"/>
-    <tableColumn id="6" name="Horas Totales" dataDxfId="3" dataCellStyle="Error">
+    <tableColumn id="6" name="Horas Totales" dataDxfId="2" dataCellStyle="Error">
       <calculatedColumnFormula>Tabla248[[#This Row],[Horas Trabajadas en Reunion]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" name="¿Completó el_x000a_Objetivo?" dataCellStyle="Note"/>
@@ -8797,7 +8982,7 @@
     <tableColumn id="3" name="Horas Trabajadas en Reunion" dataCellStyle="Entrada"/>
     <tableColumn id="4" name="Horas Autónomas" dataCellStyle="60% - Énfasis6"/>
     <tableColumn id="5" name="Justifique las horas autónomas" dataCellStyle="Note"/>
-    <tableColumn id="6" name="Horas Totales" dataDxfId="2" dataCellStyle="Error">
+    <tableColumn id="6" name="Horas Totales" dataDxfId="1" dataCellStyle="Error">
       <calculatedColumnFormula>Tabla2489[[#This Row],[Horas Trabajadas en Reunion]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" name="¿Completó el_x000a_Objetivo?" dataCellStyle="Note"/>
@@ -8838,7 +9023,7 @@
     <tableColumn id="3" name="Horas Trabajadas en Reunion" dataCellStyle="Entrada"/>
     <tableColumn id="4" name="Horas Autónomas" dataCellStyle="60% - Énfasis6"/>
     <tableColumn id="5" name="Justifique las horas autónomas" dataCellStyle="Note"/>
-    <tableColumn id="6" name="Horas Totales" dataDxfId="1" dataCellStyle="Error">
+    <tableColumn id="6" name="Horas Totales" dataDxfId="0" dataCellStyle="Error">
       <calculatedColumnFormula>Tabla248910[[#This Row],[Horas Trabajadas en Reunion]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" name="¿Completó el_x000a_Objetivo?" dataCellStyle="Note"/>
@@ -8912,60 +9097,75 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="K3:P5" totalsRowShown="0">
-  <autoFilter ref="K3:P5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Tabla612" displayName="Tabla612" ref="Q53:V55" totalsRowShown="0">
+  <autoFilter ref="Q53:V55"/>
   <tableColumns count="6">
-    <tableColumn id="7" name="Tipo"/>
-    <tableColumn id="1" name="Horas Iniciales" dataDxfId="0">
-      <calculatedColumnFormula>Tabla18[[#This Row],[Horas Totales 
-Asignadas por Tarea]]+C5+C6+C7+C8+C9+C10+C11</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="2" name="Semana 1">
-      <calculatedColumnFormula>L4-Tabla18[[#This Row],[Primera Semana]]-D5</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="3" name="Semana 2">
-      <calculatedColumnFormula>M4-E6-E7</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="4" name="Semana 3">
-      <calculatedColumnFormula>N4-F8-F9</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="5" name="Semana 4">
-      <calculatedColumnFormula>O4-G10-G11</calculatedColumnFormula>
-    </tableColumn>
+    <tableColumn id="6" name="Tipo"/>
+    <tableColumn id="1" name="Horas Iniciales"/>
+    <tableColumn id="2" name="Semana 1"/>
+    <tableColumn id="3" name="Semana 2"/>
+    <tableColumn id="4" name="Semana 3"/>
+    <tableColumn id="5" name="Semana 4"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleDark4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="K14:P16" totalsRowShown="0">
-  <autoFilter ref="K14:P16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabla6" displayName="Tabla6" ref="Q48:V50" totalsRowShown="0">
+  <autoFilter ref="Q48:V50"/>
   <tableColumns count="6">
     <tableColumn id="6" name="Tipo"/>
     <tableColumn id="1" name="Horas Iniciales">
-      <calculatedColumnFormula>Tabla1820[[#This Row],[Horas Totales 
-Asignadas por Tarea]]+C23+C16+C17+C18+C19+C20+C21+C22</calculatedColumnFormula>
+      <calculatedColumnFormula>Tabla182023[[#This Row],[Horas Totales 
+Asignadas por Tarea]]+C50+C51+C52+C53+C54+C55+C56</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" name="Semana 1">
-      <calculatedColumnFormula>L15--Tabla1820[[#This Row],[Primera Semana]]-D16-D17</calculatedColumnFormula>
+      <calculatedColumnFormula>R49-Tabla182023[[#This Row],[Primera Semana]]-D50</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" name="Semana 2">
-      <calculatedColumnFormula>M15-E18-E19</calculatedColumnFormula>
+      <calculatedColumnFormula>S49-E51-E52</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" name="Semana 3">
-      <calculatedColumnFormula>N15-F21-F20</calculatedColumnFormula>
+      <calculatedColumnFormula>T49-F53-F54</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" name="Semana 4">
-      <calculatedColumnFormula>O15-G23-G22</calculatedColumnFormula>
+      <calculatedColumnFormula>U49-G55-G56</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabla4" displayName="Tabla4" ref="K26:P28" totalsRowShown="0">
-  <autoFilter ref="K26:P28"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabla5" displayName="Tabla5" ref="Q37:V39" totalsRowShown="0">
+  <autoFilter ref="Q37:V39"/>
+  <tableColumns count="6">
+    <tableColumn id="6" name="Tipo"/>
+    <tableColumn id="1" name="Horas Iniciales">
+      <calculatedColumnFormula>Tabla182022[[#This Row],[Horas Totales 
+Asignadas por Tarea]]+C39+C40+C41+C42+C43+C44+C45</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" name="Semana 1">
+      <calculatedColumnFormula>R38-Tabla182022[[#This Row],[Primera Semana]]-D39</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" name="Semana 2">
+      <calculatedColumnFormula>S38-E40-E41</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" name="Semana 3">
+      <calculatedColumnFormula>T38-F42-F43</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" name="Semana 4">
+      <calculatedColumnFormula>U38-G44-G45</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabla4" displayName="Tabla4" ref="Q26:V28" totalsRowShown="0">
+  <autoFilter ref="Q26:V28"/>
   <tableColumns count="6">
     <tableColumn id="7" name="Tipo"/>
     <tableColumn id="1" name="Horas Iniciales">
@@ -8973,45 +9173,19 @@
 Asignadas por Tarea]]+C28+C29+C30+C31+C32+C33+C34</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" name="Semana 1">
-      <calculatedColumnFormula>L27-Tabla182021[[#This Row],[Primera Semana]]-D28</calculatedColumnFormula>
+      <calculatedColumnFormula>R27-Tabla182021[[#This Row],[Primera Semana]]-D28</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" name="Semana 2">
-      <calculatedColumnFormula>M27-E29-E30</calculatedColumnFormula>
+      <calculatedColumnFormula>S27-E29-E30</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" name="Semana 3">
-      <calculatedColumnFormula>N27-F31-F32</calculatedColumnFormula>
+      <calculatedColumnFormula>T27-F31-F32</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" name="Semana 4">
-      <calculatedColumnFormula>O27-G33-G34</calculatedColumnFormula>
+      <calculatedColumnFormula>U27-G33-G34</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabla5" displayName="Tabla5" ref="K37:P39" totalsRowShown="0">
-  <autoFilter ref="K37:P39"/>
-  <tableColumns count="6">
-    <tableColumn id="6" name="Tipo"/>
-    <tableColumn id="1" name="Horas Iniciales">
-      <calculatedColumnFormula>Tabla182022[[#This Row],[Horas Totales 
-Asignadas por Tarea]]+C39+C40+C41+C42+C43+C44+C45</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="2" name="Semana 1">
-      <calculatedColumnFormula>L38-Tabla182022[[#This Row],[Primera Semana]]-D39</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="3" name="Semana 2">
-      <calculatedColumnFormula>M38-E40-E41</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="4" name="Semana 3">
-      <calculatedColumnFormula>N38-F42-F43</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="5" name="Semana 4">
-      <calculatedColumnFormula>O38-G44-G45</calculatedColumnFormula>
-    </tableColumn>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -9278,10 +9452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:P65"/>
+  <dimension ref="A3:V56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E59" sqref="E59"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -9304,7 +9478,7 @@
     <col min="16" max="16" width="16.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:16" ht="26.25">
+    <row r="3" spans="1:22" ht="26.25">
       <c r="A3" s="61" t="s">
         <v>39</v>
       </c>
@@ -9332,26 +9506,26 @@
       <c r="I3" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="K3" t="s">
+      <c r="Q3" t="s">
         <v>50</v>
       </c>
-      <c r="L3" t="s">
+      <c r="R3" t="s">
         <v>45</v>
       </c>
-      <c r="M3" t="s">
+      <c r="S3" t="s">
         <v>47</v>
       </c>
-      <c r="N3" t="s">
+      <c r="T3" t="s">
         <v>46</v>
       </c>
-      <c r="O3" t="s">
+      <c r="U3" t="s">
         <v>48</v>
       </c>
-      <c r="P3" t="s">
+      <c r="V3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="15">
+    <row r="4" spans="1:22" ht="15">
       <c r="A4" s="64" t="s">
         <v>41</v>
       </c>
@@ -9369,38 +9543,38 @@
       <c r="F4" s="60"/>
       <c r="G4" s="60"/>
       <c r="H4" s="67">
-        <f t="shared" ref="H4:H11" si="0">D4+E4+F4+G4</f>
+        <f>D4+E4+F4+G4</f>
         <v>1.25</v>
       </c>
       <c r="I4" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="K4" t="s">
+      <c r="Q4" t="s">
         <v>51</v>
       </c>
-      <c r="L4">
+      <c r="R4">
         <f>Tabla18[[#This Row],[Horas Totales 
 Asignadas por Tarea]]+C5+C6+C7+C8+C9+C10+C11</f>
         <v>5</v>
       </c>
-      <c r="M4">
-        <f>L4-Tabla18[[#This Row],[Primera Semana]]-D5</f>
+      <c r="S4">
+        <f>R4-Tabla18[[#This Row],[Primera Semana]]-D5</f>
         <v>3.75</v>
       </c>
-      <c r="N4">
-        <f>M4-E6-E7</f>
+      <c r="T4">
+        <f>S4-E6-E7</f>
         <v>3.75</v>
       </c>
-      <c r="O4">
-        <f>N4-F8-F9</f>
+      <c r="U4">
+        <f>T4-F8-F9</f>
         <v>3.75</v>
       </c>
-      <c r="P4">
-        <f>O4-G10-G11</f>
+      <c r="V4">
+        <f>U4-G10-G11</f>
         <v>3.75</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="15">
+    <row r="5" spans="1:22" ht="15">
       <c r="A5" s="69"/>
       <c r="B5" s="46" t="s">
         <v>7</v>
@@ -9416,35 +9590,35 @@
       <c r="F5" s="47"/>
       <c r="G5" s="47"/>
       <c r="H5" s="71">
-        <f t="shared" si="0"/>
+        <f>D5+E5+F5+G5</f>
         <v>0</v>
       </c>
       <c r="I5" s="72"/>
-      <c r="K5" t="s">
+      <c r="Q5" t="s">
         <v>52</v>
       </c>
-      <c r="L5">
-        <f>L4</f>
+      <c r="R5">
+        <f>R4</f>
         <v>5</v>
       </c>
-      <c r="M5">
+      <c r="S5">
         <f>Tabla1[[#This Row],[Horas Iniciales]]-(Tabla1[[#This Row],[Horas Iniciales]]/4)</f>
         <v>3.75</v>
       </c>
-      <c r="N5">
+      <c r="T5">
         <f>Tabla1[[#This Row],[Semana 1]]-(Tabla1[[#This Row],[Horas Iniciales]]/4)</f>
         <v>2.5</v>
       </c>
-      <c r="O5">
+      <c r="U5">
         <f>Tabla1[[#This Row],[Semana 2]]-(Tabla1[[#This Row],[Horas Iniciales]]/4)</f>
         <v>1.25</v>
       </c>
-      <c r="P5">
+      <c r="V5">
         <f>Tabla1[[#This Row],[Semana 3]]-(Tabla1[[#This Row],[Horas Iniciales]]/4)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="15">
+    <row r="6" spans="1:22" ht="15">
       <c r="A6" s="69"/>
       <c r="B6" s="51"/>
       <c r="C6" s="70"/>
@@ -9453,12 +9627,12 @@
       <c r="F6" s="54"/>
       <c r="G6" s="54"/>
       <c r="H6" s="71">
-        <f t="shared" si="0"/>
+        <f>D6+E6+F6+G6</f>
         <v>0</v>
       </c>
       <c r="I6" s="73"/>
     </row>
-    <row r="7" spans="1:16" ht="15">
+    <row r="7" spans="1:22" ht="15">
       <c r="A7" s="69"/>
       <c r="B7" s="49"/>
       <c r="C7" s="70"/>
@@ -9467,12 +9641,12 @@
       <c r="F7" s="47"/>
       <c r="G7" s="47"/>
       <c r="H7" s="71">
-        <f t="shared" si="0"/>
+        <f>D7+E7+F7+G7</f>
         <v>0</v>
       </c>
       <c r="I7" s="72"/>
     </row>
-    <row r="8" spans="1:16" ht="15">
+    <row r="8" spans="1:22" ht="15">
       <c r="A8" s="69"/>
       <c r="B8" s="52"/>
       <c r="C8" s="70"/>
@@ -9481,12 +9655,12 @@
       <c r="F8" s="52"/>
       <c r="G8" s="47"/>
       <c r="H8" s="71">
-        <f t="shared" si="0"/>
+        <f>D8+E8+F8+G8</f>
         <v>0</v>
       </c>
       <c r="I8" s="72"/>
     </row>
-    <row r="9" spans="1:16" ht="15">
+    <row r="9" spans="1:22" ht="15">
       <c r="A9" s="69"/>
       <c r="B9" s="52"/>
       <c r="C9" s="70"/>
@@ -9495,12 +9669,12 @@
       <c r="F9" s="52"/>
       <c r="G9" s="47"/>
       <c r="H9" s="71">
-        <f t="shared" si="0"/>
+        <f>D9+E9+F9+G9</f>
         <v>0</v>
       </c>
       <c r="I9" s="72"/>
     </row>
-    <row r="10" spans="1:16" ht="15">
+    <row r="10" spans="1:22" ht="15">
       <c r="A10" s="69"/>
       <c r="B10" s="53"/>
       <c r="C10" s="70"/>
@@ -9509,12 +9683,12 @@
       <c r="F10" s="47"/>
       <c r="G10" s="53"/>
       <c r="H10" s="71">
-        <f t="shared" si="0"/>
+        <f>D10+E10+F10+G10</f>
         <v>0</v>
       </c>
       <c r="I10" s="72"/>
     </row>
-    <row r="11" spans="1:16" ht="15">
+    <row r="11" spans="1:22" ht="15">
       <c r="A11" s="74"/>
       <c r="B11" s="75"/>
       <c r="C11" s="76"/>
@@ -9523,12 +9697,12 @@
       <c r="F11" s="77"/>
       <c r="G11" s="75"/>
       <c r="H11" s="78">
-        <f t="shared" si="0"/>
+        <f>D11+E11+F11+G11</f>
         <v>0</v>
       </c>
       <c r="I11" s="79"/>
     </row>
-    <row r="14" spans="1:16" ht="26.25">
+    <row r="14" spans="1:22" ht="26.25">
       <c r="A14" s="43" t="s">
         <v>39</v>
       </c>
@@ -9556,26 +9730,26 @@
       <c r="I14" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="K14" t="s">
+      <c r="Q14" t="s">
         <v>50</v>
       </c>
-      <c r="L14" t="s">
+      <c r="R14" t="s">
         <v>45</v>
       </c>
-      <c r="M14" t="s">
+      <c r="S14" t="s">
         <v>47</v>
       </c>
-      <c r="N14" t="s">
+      <c r="T14" t="s">
         <v>46</v>
       </c>
-      <c r="O14" t="s">
+      <c r="U14" t="s">
         <v>48</v>
       </c>
-      <c r="P14" t="s">
+      <c r="V14" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="15">
+    <row r="15" spans="1:22" ht="15">
       <c r="A15" s="50" t="s">
         <v>40</v>
       </c>
@@ -9593,36 +9767,36 @@
       <c r="F15" s="47"/>
       <c r="G15" s="47"/>
       <c r="H15" s="71">
-        <f t="shared" ref="H15:H23" si="1">D15+E15+F15+G15</f>
+        <f>D15+E15+F15+G15</f>
         <v>0</v>
       </c>
       <c r="I15" s="56"/>
-      <c r="K15" t="s">
+      <c r="Q15" t="s">
         <v>51</v>
       </c>
-      <c r="L15">
+      <c r="R15">
         <f>Tabla1820[[#This Row],[Horas Totales 
 Asignadas por Tarea]]+C23+C16+C17+C18+C19+C20+C21+C22</f>
         <v>7</v>
       </c>
-      <c r="M15">
-        <f>L15--Tabla1820[[#This Row],[Primera Semana]]-D16-D17</f>
+      <c r="S15">
+        <f>R15--Tabla1820[[#This Row],[Primera Semana]]-D16-D17</f>
         <v>5.5</v>
       </c>
-      <c r="N15">
-        <f>M15-E18-E19</f>
+      <c r="T15">
+        <f>S15-E18-E19</f>
         <v>5.5</v>
       </c>
-      <c r="O15">
-        <f>N15-F21-F20</f>
+      <c r="U15">
+        <f>T15-F21-F20</f>
         <v>5.5</v>
       </c>
-      <c r="P15">
-        <f>O15-G23-G22</f>
+      <c r="V15">
+        <f>U15-G23-G22</f>
         <v>5.5</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="15">
+    <row r="16" spans="1:22" ht="15">
       <c r="A16" s="50"/>
       <c r="B16" s="46" t="s">
         <v>7</v>
@@ -9638,35 +9812,35 @@
       <c r="F16" s="47"/>
       <c r="G16" s="47"/>
       <c r="H16" s="71">
-        <f t="shared" si="1"/>
+        <f>D16+E16+F16+G16</f>
         <v>0</v>
       </c>
       <c r="I16" s="56"/>
-      <c r="K16" t="s">
+      <c r="Q16" t="s">
         <v>52</v>
       </c>
-      <c r="L16">
-        <f>L15</f>
+      <c r="R16">
+        <f>R15</f>
         <v>7</v>
       </c>
-      <c r="M16">
+      <c r="S16">
         <f>Tabla2[[#This Row],[Horas Iniciales]]-(Tabla2[[#This Row],[Horas Iniciales]]/4)</f>
         <v>5.25</v>
       </c>
-      <c r="N16">
+      <c r="T16">
         <f>Tabla2[[#This Row],[Semana 1]]-(Tabla2[[#This Row],[Horas Iniciales]]/4)</f>
         <v>3.5</v>
       </c>
-      <c r="O16">
+      <c r="U16">
         <f>Tabla2[[#This Row],[Semana 2]]-(Tabla2[[#This Row],[Horas Iniciales]]/4)</f>
         <v>1.75</v>
       </c>
-      <c r="P16">
+      <c r="V16">
         <f>Tabla2[[#This Row],[Semana 3]]-(Tabla2[[#This Row],[Horas Iniciales]]/4)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="15">
+    <row r="17" spans="1:22" ht="15">
       <c r="A17" s="50"/>
       <c r="B17" s="86" t="s">
         <v>14</v>
@@ -9682,14 +9856,14 @@
       <c r="F17" s="89"/>
       <c r="G17" s="89"/>
       <c r="H17" s="90">
-        <f t="shared" si="1"/>
+        <f>D17+E17+F17+G17</f>
         <v>1.5</v>
       </c>
       <c r="I17" s="91" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="15">
+    <row r="18" spans="1:22" ht="15">
       <c r="A18" s="50"/>
       <c r="B18" s="51"/>
       <c r="C18" s="70"/>
@@ -9698,12 +9872,12 @@
       <c r="F18" s="54"/>
       <c r="G18" s="54"/>
       <c r="H18" s="71">
-        <f t="shared" si="1"/>
+        <f>D18+E18+F18+G18</f>
         <v>0</v>
       </c>
       <c r="I18" s="57"/>
     </row>
-    <row r="19" spans="1:16" ht="15">
+    <row r="19" spans="1:22" ht="15">
       <c r="A19" s="50"/>
       <c r="B19" s="49"/>
       <c r="C19" s="70"/>
@@ -9712,12 +9886,12 @@
       <c r="F19" s="47"/>
       <c r="G19" s="47"/>
       <c r="H19" s="71">
-        <f t="shared" si="1"/>
+        <f>D19+E19+F19+G19</f>
         <v>0</v>
       </c>
       <c r="I19" s="56"/>
     </row>
-    <row r="20" spans="1:16" ht="15">
+    <row r="20" spans="1:22" ht="15">
       <c r="A20" s="50"/>
       <c r="B20" s="52"/>
       <c r="C20" s="70"/>
@@ -9726,12 +9900,12 @@
       <c r="F20" s="52"/>
       <c r="G20" s="47"/>
       <c r="H20" s="71">
-        <f t="shared" si="1"/>
+        <f>D20+E20+F20+G20</f>
         <v>0</v>
       </c>
       <c r="I20" s="56"/>
     </row>
-    <row r="21" spans="1:16" ht="15">
+    <row r="21" spans="1:22" ht="15">
       <c r="A21" s="50"/>
       <c r="B21" s="52"/>
       <c r="C21" s="70"/>
@@ -9740,12 +9914,12 @@
       <c r="F21" s="52"/>
       <c r="G21" s="47"/>
       <c r="H21" s="71">
-        <f t="shared" si="1"/>
+        <f>D21+E21+F21+G21</f>
         <v>0</v>
       </c>
       <c r="I21" s="56"/>
     </row>
-    <row r="22" spans="1:16" ht="15">
+    <row r="22" spans="1:22" ht="15">
       <c r="A22" s="50"/>
       <c r="B22" s="53"/>
       <c r="C22" s="70"/>
@@ -9754,12 +9928,12 @@
       <c r="F22" s="47"/>
       <c r="G22" s="53"/>
       <c r="H22" s="71">
-        <f t="shared" si="1"/>
+        <f>D22+E22+F22+G22</f>
         <v>0</v>
       </c>
       <c r="I22" s="56"/>
     </row>
-    <row r="23" spans="1:16" ht="15">
+    <row r="23" spans="1:22" ht="15">
       <c r="A23" s="50"/>
       <c r="B23" s="81"/>
       <c r="C23" s="17"/>
@@ -9768,12 +9942,12 @@
       <c r="F23" s="54"/>
       <c r="G23" s="81"/>
       <c r="H23" s="71">
-        <f t="shared" si="1"/>
+        <f>D23+E23+F23+G23</f>
         <v>0</v>
       </c>
       <c r="I23" s="57"/>
     </row>
-    <row r="26" spans="1:16" ht="26.25">
+    <row r="26" spans="1:22" ht="26.25">
       <c r="A26" s="43" t="s">
         <v>39</v>
       </c>
@@ -9801,26 +9975,26 @@
       <c r="I26" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="K26" t="s">
+      <c r="Q26" t="s">
         <v>50</v>
       </c>
-      <c r="L26" t="s">
+      <c r="R26" t="s">
         <v>45</v>
       </c>
-      <c r="M26" t="s">
+      <c r="S26" t="s">
         <v>47</v>
       </c>
-      <c r="N26" t="s">
+      <c r="T26" t="s">
         <v>46</v>
       </c>
-      <c r="O26" t="s">
+      <c r="U26" t="s">
         <v>48</v>
       </c>
-      <c r="P26" t="s">
+      <c r="V26" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="15">
+    <row r="27" spans="1:22" ht="15">
       <c r="A27" s="50" t="s">
         <v>42</v>
       </c>
@@ -9838,38 +10012,38 @@
       <c r="F27" s="47"/>
       <c r="G27" s="47"/>
       <c r="H27" s="71">
-        <f t="shared" ref="H27:H34" si="2">D27+E27+F27+G27</f>
+        <f>D27+E27+F27+G27</f>
         <v>1.5</v>
       </c>
       <c r="I27" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="K27" t="s">
+      <c r="Q27" t="s">
         <v>51</v>
       </c>
-      <c r="L27">
+      <c r="R27">
         <f>Tabla182021[[#This Row],[Horas Totales 
 Asignadas por Tarea]]+C28+C29+C30+C31+C32+C33+C34</f>
         <v>5</v>
       </c>
-      <c r="M27">
-        <f>L27-Tabla182021[[#This Row],[Primera Semana]]-D28</f>
+      <c r="S27">
+        <f>R27-Tabla182021[[#This Row],[Primera Semana]]-D28</f>
         <v>3.5</v>
       </c>
-      <c r="N27">
-        <f>M27-E29-E30</f>
+      <c r="T27">
+        <f>S27-E29-E30</f>
         <v>3.5</v>
       </c>
-      <c r="O27">
-        <f>N27-F31-F32</f>
+      <c r="U27">
+        <f>T27-F31-F32</f>
         <v>3.5</v>
       </c>
-      <c r="P27">
-        <f>O27-G33-G34</f>
+      <c r="V27">
+        <f>U27-G33-G34</f>
         <v>3.5</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="15">
+    <row r="28" spans="1:22" ht="15">
       <c r="A28" s="50"/>
       <c r="B28" s="46" t="s">
         <v>7</v>
@@ -9885,35 +10059,35 @@
       <c r="F28" s="47"/>
       <c r="G28" s="47"/>
       <c r="H28" s="71">
-        <f t="shared" si="2"/>
+        <f>D28+E28+F28+G28</f>
         <v>0</v>
       </c>
       <c r="I28" s="56"/>
-      <c r="K28" t="s">
+      <c r="Q28" t="s">
         <v>52</v>
       </c>
-      <c r="L28">
-        <f>L27</f>
+      <c r="R28">
+        <f>R27</f>
         <v>5</v>
       </c>
-      <c r="M28">
+      <c r="S28">
         <f>Tabla4[[#This Row],[Horas Iniciales]]-(Tabla4[[#This Row],[Horas Iniciales]]/4)</f>
         <v>3.75</v>
       </c>
-      <c r="N28">
+      <c r="T28">
         <f>Tabla4[[#This Row],[Semana 1]]-(Tabla4[[#This Row],[Horas Iniciales]]/4)</f>
         <v>2.5</v>
       </c>
-      <c r="O28">
+      <c r="U28">
         <f>Tabla4[[#This Row],[Semana 2]]-(Tabla4[[#This Row],[Horas Iniciales]]/4)</f>
         <v>1.25</v>
       </c>
-      <c r="P28">
+      <c r="V28">
         <f>Tabla4[[#This Row],[Semana 3]]-(Tabla4[[#This Row],[Horas Iniciales]]/4)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="15">
+    <row r="29" spans="1:22" ht="15">
       <c r="A29" s="50"/>
       <c r="B29" s="51"/>
       <c r="C29" s="70"/>
@@ -9922,12 +10096,12 @@
       <c r="F29" s="54"/>
       <c r="G29" s="54"/>
       <c r="H29" s="71">
-        <f t="shared" si="2"/>
+        <f>D29+E29+F29+G29</f>
         <v>0</v>
       </c>
       <c r="I29" s="57"/>
     </row>
-    <row r="30" spans="1:16" ht="15">
+    <row r="30" spans="1:22" ht="15">
       <c r="A30" s="50"/>
       <c r="B30" s="49"/>
       <c r="C30" s="70"/>
@@ -9936,12 +10110,12 @@
       <c r="F30" s="47"/>
       <c r="G30" s="47"/>
       <c r="H30" s="71">
-        <f t="shared" si="2"/>
+        <f>D30+E30+F30+G30</f>
         <v>0</v>
       </c>
       <c r="I30" s="56"/>
     </row>
-    <row r="31" spans="1:16" ht="15">
+    <row r="31" spans="1:22" ht="15">
       <c r="A31" s="50"/>
       <c r="B31" s="52"/>
       <c r="C31" s="70"/>
@@ -9950,12 +10124,12 @@
       <c r="F31" s="52"/>
       <c r="G31" s="47"/>
       <c r="H31" s="71">
-        <f t="shared" si="2"/>
+        <f>D31+E31+F31+G31</f>
         <v>0</v>
       </c>
       <c r="I31" s="56"/>
     </row>
-    <row r="32" spans="1:16" ht="15">
+    <row r="32" spans="1:22" ht="15">
       <c r="A32" s="50"/>
       <c r="B32" s="52"/>
       <c r="C32" s="70"/>
@@ -9964,12 +10138,12 @@
       <c r="F32" s="52"/>
       <c r="G32" s="47"/>
       <c r="H32" s="71">
-        <f t="shared" si="2"/>
+        <f>D32+E32+F32+G32</f>
         <v>0</v>
       </c>
       <c r="I32" s="56"/>
     </row>
-    <row r="33" spans="1:16" ht="15">
+    <row r="33" spans="1:22" ht="15">
       <c r="A33" s="50"/>
       <c r="B33" s="53"/>
       <c r="C33" s="70"/>
@@ -9978,12 +10152,12 @@
       <c r="F33" s="47"/>
       <c r="G33" s="53"/>
       <c r="H33" s="71">
-        <f t="shared" si="2"/>
+        <f>D33+E33+F33+G33</f>
         <v>0</v>
       </c>
       <c r="I33" s="56"/>
     </row>
-    <row r="34" spans="1:16" ht="15">
+    <row r="34" spans="1:22" ht="15">
       <c r="A34" s="50"/>
       <c r="B34" s="81"/>
       <c r="C34" s="17"/>
@@ -9992,12 +10166,12 @@
       <c r="F34" s="54"/>
       <c r="G34" s="81"/>
       <c r="H34" s="71">
-        <f t="shared" si="2"/>
+        <f>D34+E34+F34+G34</f>
         <v>0</v>
       </c>
       <c r="I34" s="57"/>
     </row>
-    <row r="37" spans="1:16" ht="26.25">
+    <row r="37" spans="1:22" ht="26.25">
       <c r="A37" s="43" t="s">
         <v>39</v>
       </c>
@@ -10025,26 +10199,26 @@
       <c r="I37" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="K37" t="s">
+      <c r="Q37" t="s">
         <v>50</v>
       </c>
-      <c r="L37" t="s">
+      <c r="R37" t="s">
         <v>45</v>
       </c>
-      <c r="M37" t="s">
+      <c r="S37" t="s">
         <v>47</v>
       </c>
-      <c r="N37" t="s">
+      <c r="T37" t="s">
         <v>46</v>
       </c>
-      <c r="O37" t="s">
+      <c r="U37" t="s">
         <v>48</v>
       </c>
-      <c r="P37" t="s">
+      <c r="V37" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="38" spans="1:16" ht="15">
+    <row r="38" spans="1:22" ht="15">
       <c r="A38" s="50" t="s">
         <v>43</v>
       </c>
@@ -10062,36 +10236,36 @@
       <c r="F38" s="47"/>
       <c r="G38" s="47"/>
       <c r="H38" s="71">
-        <f t="shared" ref="H38:H45" si="3">D38+E38+F38+G38</f>
+        <f>D38+E38+F38+G38</f>
         <v>1</v>
       </c>
       <c r="I38" s="56"/>
-      <c r="K38" t="s">
+      <c r="Q38" t="s">
         <v>51</v>
       </c>
-      <c r="L38">
+      <c r="R38">
         <f>Tabla182022[[#This Row],[Horas Totales 
 Asignadas por Tarea]]+C39+C40+C41+C42+C43+C44+C45</f>
         <v>5</v>
       </c>
-      <c r="M38">
-        <f>L38-Tabla182022[[#This Row],[Primera Semana]]-D39</f>
+      <c r="S38">
+        <f>R38-Tabla182022[[#This Row],[Primera Semana]]-D39</f>
         <v>4</v>
       </c>
-      <c r="N38">
-        <f>M38-E40-E41</f>
+      <c r="T38">
+        <f>S38-E40-E41</f>
         <v>4</v>
       </c>
-      <c r="O38">
-        <f>N38-F42-F43</f>
+      <c r="U38">
+        <f>T38-F42-F43</f>
         <v>4</v>
       </c>
-      <c r="P38">
-        <f>O38-G44-G45</f>
+      <c r="V38">
+        <f>U38-G44-G45</f>
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:16" ht="15">
+    <row r="39" spans="1:22" ht="15">
       <c r="A39" s="50"/>
       <c r="B39" s="46" t="s">
         <v>7</v>
@@ -10107,35 +10281,35 @@
       <c r="F39" s="47"/>
       <c r="G39" s="47"/>
       <c r="H39" s="71">
-        <f t="shared" si="3"/>
+        <f>D39+E39+F39+G39</f>
         <v>0</v>
       </c>
       <c r="I39" s="56"/>
-      <c r="K39" t="s">
+      <c r="Q39" t="s">
         <v>52</v>
       </c>
-      <c r="L39">
-        <f>L38</f>
+      <c r="R39">
+        <f>R38</f>
         <v>5</v>
       </c>
-      <c r="M39">
+      <c r="S39">
         <f>Tabla5[[#This Row],[Horas Iniciales]]-(Tabla5[[#This Row],[Horas Iniciales]]/4)</f>
         <v>3.75</v>
       </c>
-      <c r="N39">
+      <c r="T39">
         <f>Tabla5[[#This Row],[Semana 1]]-(Tabla5[[#This Row],[Horas Iniciales]]/4)</f>
         <v>2.5</v>
       </c>
-      <c r="O39">
+      <c r="U39">
         <f>Tabla5[[#This Row],[Semana 2]]-(Tabla5[[#This Row],[Horas Iniciales]]/4)</f>
         <v>1.25</v>
       </c>
-      <c r="P39">
+      <c r="V39">
         <f>Tabla5[[#This Row],[Semana 3]]-(Tabla5[[#This Row],[Horas Iniciales]]/4)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:16" ht="15">
+    <row r="40" spans="1:22" ht="15">
       <c r="A40" s="50"/>
       <c r="B40" s="51"/>
       <c r="C40" s="70"/>
@@ -10144,12 +10318,12 @@
       <c r="F40" s="54"/>
       <c r="G40" s="54"/>
       <c r="H40" s="71">
-        <f t="shared" si="3"/>
+        <f>D40+E40+F40+G40</f>
         <v>0</v>
       </c>
       <c r="I40" s="57"/>
     </row>
-    <row r="41" spans="1:16" ht="15">
+    <row r="41" spans="1:22" ht="15">
       <c r="A41" s="50"/>
       <c r="B41" s="49"/>
       <c r="C41" s="70"/>
@@ -10158,12 +10332,12 @@
       <c r="F41" s="47"/>
       <c r="G41" s="47"/>
       <c r="H41" s="71">
-        <f t="shared" si="3"/>
+        <f>D41+E41+F41+G41</f>
         <v>0</v>
       </c>
       <c r="I41" s="56"/>
     </row>
-    <row r="42" spans="1:16" ht="15">
+    <row r="42" spans="1:22" ht="15">
       <c r="A42" s="50"/>
       <c r="B42" s="52"/>
       <c r="C42" s="70"/>
@@ -10172,12 +10346,12 @@
       <c r="F42" s="52"/>
       <c r="G42" s="47"/>
       <c r="H42" s="71">
-        <f t="shared" si="3"/>
+        <f>D42+E42+F42+G42</f>
         <v>0</v>
       </c>
       <c r="I42" s="56"/>
     </row>
-    <row r="43" spans="1:16" ht="15">
+    <row r="43" spans="1:22" ht="15">
       <c r="A43" s="50"/>
       <c r="B43" s="52"/>
       <c r="C43" s="70"/>
@@ -10186,12 +10360,12 @@
       <c r="F43" s="52"/>
       <c r="G43" s="47"/>
       <c r="H43" s="71">
-        <f t="shared" si="3"/>
+        <f>D43+E43+F43+G43</f>
         <v>0</v>
       </c>
       <c r="I43" s="56"/>
     </row>
-    <row r="44" spans="1:16" ht="15">
+    <row r="44" spans="1:22" ht="15">
       <c r="A44" s="50"/>
       <c r="B44" s="53"/>
       <c r="C44" s="70"/>
@@ -10200,12 +10374,12 @@
       <c r="F44" s="47"/>
       <c r="G44" s="53"/>
       <c r="H44" s="71">
-        <f t="shared" si="3"/>
+        <f>D44+E44+F44+G44</f>
         <v>0</v>
       </c>
       <c r="I44" s="56"/>
     </row>
-    <row r="45" spans="1:16" ht="15">
+    <row r="45" spans="1:22" ht="15">
       <c r="A45" s="50"/>
       <c r="B45" s="81"/>
       <c r="C45" s="17"/>
@@ -10214,12 +10388,12 @@
       <c r="F45" s="54"/>
       <c r="G45" s="81"/>
       <c r="H45" s="71">
-        <f t="shared" si="3"/>
+        <f>D45+E45+F45+G45</f>
         <v>0</v>
       </c>
       <c r="I45" s="57"/>
     </row>
-    <row r="48" spans="1:16" ht="26.25">
+    <row r="48" spans="1:22" ht="26.25">
       <c r="A48" s="43" t="s">
         <v>39</v>
       </c>
@@ -10247,26 +10421,26 @@
       <c r="I48" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="K48" t="s">
+      <c r="Q48" t="s">
         <v>50</v>
       </c>
-      <c r="L48" t="s">
+      <c r="R48" t="s">
         <v>45</v>
       </c>
-      <c r="M48" t="s">
+      <c r="S48" t="s">
         <v>47</v>
       </c>
-      <c r="N48" t="s">
+      <c r="T48" t="s">
         <v>46</v>
       </c>
-      <c r="O48" t="s">
+      <c r="U48" t="s">
         <v>48</v>
       </c>
-      <c r="P48" t="s">
+      <c r="V48" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="49" spans="1:16" ht="15">
+    <row r="49" spans="1:22" ht="15">
       <c r="A49" s="50" t="s">
         <v>44</v>
       </c>
@@ -10284,36 +10458,36 @@
       <c r="F49" s="47"/>
       <c r="G49" s="47"/>
       <c r="H49" s="71">
-        <f t="shared" ref="H49:H56" si="4">D49+E49+F49+G49</f>
+        <f t="shared" ref="H49:H56" si="0">D49+E49+F49+G49</f>
         <v>1.25</v>
       </c>
       <c r="I49" s="56"/>
-      <c r="K49" t="s">
+      <c r="Q49" t="s">
         <v>51</v>
       </c>
-      <c r="L49">
+      <c r="R49">
         <f>Tabla182023[[#This Row],[Horas Totales 
 Asignadas por Tarea]]+C50+C51+C52+C53+C54+C55+C56</f>
         <v>5</v>
       </c>
-      <c r="M49">
-        <f>L49-Tabla182023[[#This Row],[Primera Semana]]-D50</f>
+      <c r="S49">
+        <f>R49-Tabla182023[[#This Row],[Primera Semana]]-D50</f>
         <v>3.75</v>
       </c>
-      <c r="N49">
-        <f>M49-E51-E52</f>
+      <c r="T49">
+        <f>S49-E51-E52</f>
         <v>3.75</v>
       </c>
-      <c r="O49">
-        <f>N49-F53-F54</f>
+      <c r="U49">
+        <f>T49-F53-F54</f>
         <v>3.75</v>
       </c>
-      <c r="P49">
-        <f>O49-G55-G56</f>
+      <c r="V49">
+        <f>U49-G55-G56</f>
         <v>3.75</v>
       </c>
     </row>
-    <row r="50" spans="1:16" ht="15">
+    <row r="50" spans="1:22" ht="15">
       <c r="A50" s="50"/>
       <c r="B50" s="46" t="s">
         <v>7</v>
@@ -10329,35 +10503,35 @@
       <c r="F50" s="47"/>
       <c r="G50" s="47"/>
       <c r="H50" s="71">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I50" s="56"/>
-      <c r="K50" t="s">
+      <c r="Q50" t="s">
         <v>52</v>
       </c>
-      <c r="L50">
-        <f>L49</f>
+      <c r="R50">
+        <f>R49</f>
         <v>5</v>
       </c>
-      <c r="M50">
+      <c r="S50">
         <f>Tabla6[[#This Row],[Horas Iniciales]]-(Tabla6[[#This Row],[Horas Iniciales]]/4)</f>
         <v>3.75</v>
       </c>
-      <c r="N50">
+      <c r="T50">
         <f>Tabla6[[#This Row],[Semana 1]]-(Tabla6[[#This Row],[Horas Iniciales]]/4)</f>
         <v>2.5</v>
       </c>
-      <c r="O50">
+      <c r="U50">
         <f>Tabla6[[#This Row],[Semana 2]]-(Tabla6[[#This Row],[Horas Iniciales]]/4)</f>
         <v>1.25</v>
       </c>
-      <c r="P50">
+      <c r="V50">
         <f>Tabla6[[#This Row],[Semana 3]]-(Tabla6[[#This Row],[Horas Iniciales]]/4)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:16" ht="15">
+    <row r="51" spans="1:22" ht="15">
       <c r="A51" s="50"/>
       <c r="B51" s="51"/>
       <c r="C51" s="70"/>
@@ -10366,12 +10540,12 @@
       <c r="F51" s="54"/>
       <c r="G51" s="54"/>
       <c r="H51" s="71">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I51" s="57"/>
     </row>
-    <row r="52" spans="1:16" ht="15">
+    <row r="52" spans="1:22" ht="15">
       <c r="A52" s="50"/>
       <c r="B52" s="49"/>
       <c r="C52" s="70"/>
@@ -10380,12 +10554,12 @@
       <c r="F52" s="47"/>
       <c r="G52" s="47"/>
       <c r="H52" s="71">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I52" s="56"/>
     </row>
-    <row r="53" spans="1:16" ht="15">
+    <row r="53" spans="1:22" ht="15">
       <c r="A53" s="50"/>
       <c r="B53" s="52"/>
       <c r="C53" s="70"/>
@@ -10394,12 +10568,30 @@
       <c r="F53" s="52"/>
       <c r="G53" s="47"/>
       <c r="H53" s="71">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I53" s="56"/>
+      <c r="Q53" t="s">
+        <v>50</v>
+      </c>
+      <c r="R53" t="s">
+        <v>45</v>
+      </c>
+      <c r="S53" t="s">
+        <v>47</v>
+      </c>
+      <c r="T53" t="s">
+        <v>46</v>
+      </c>
+      <c r="U53" t="s">
+        <v>48</v>
+      </c>
+      <c r="V53" t="s">
+        <v>49</v>
+      </c>
     </row>
-    <row r="54" spans="1:16" ht="15">
+    <row r="54" spans="1:22" ht="15">
       <c r="A54" s="50"/>
       <c r="B54" s="52"/>
       <c r="C54" s="70"/>
@@ -10408,12 +10600,35 @@
       <c r="F54" s="52"/>
       <c r="G54" s="47"/>
       <c r="H54" s="71">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I54" s="56"/>
+      <c r="Q54" t="s">
+        <v>51</v>
+      </c>
+      <c r="R54">
+        <f>R49+R38+R27+R15+R4</f>
+        <v>27</v>
+      </c>
+      <c r="S54">
+        <f>S49+S38+S27+S15+S4</f>
+        <v>20.5</v>
+      </c>
+      <c r="T54">
+        <f>T49+T38+T27+T15+T4</f>
+        <v>20.5</v>
+      </c>
+      <c r="U54">
+        <f>U49+U38+U27+U15+U4</f>
+        <v>20.5</v>
+      </c>
+      <c r="V54">
+        <f>V49+V38+V27+V15+V4</f>
+        <v>20.5</v>
+      </c>
     </row>
-    <row r="55" spans="1:16" ht="15">
+    <row r="55" spans="1:22" ht="15">
       <c r="A55" s="50"/>
       <c r="B55" s="53"/>
       <c r="C55" s="70"/>
@@ -10422,12 +10637,35 @@
       <c r="F55" s="47"/>
       <c r="G55" s="53"/>
       <c r="H55" s="71">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I55" s="56"/>
+      <c r="Q55" t="s">
+        <v>52</v>
+      </c>
+      <c r="R55">
+        <f>R54</f>
+        <v>27</v>
+      </c>
+      <c r="S55">
+        <f>Tabla612[[#This Row],[Horas Iniciales]]-(Tabla612[[#This Row],[Horas Iniciales]]/4)</f>
+        <v>20.25</v>
+      </c>
+      <c r="T55">
+        <f>Tabla612[[#This Row],[Semana 1]]-(Tabla612[[#This Row],[Horas Iniciales]]/4)</f>
+        <v>13.5</v>
+      </c>
+      <c r="U55">
+        <f>Tabla612[[#This Row],[Semana 2]]-(Tabla612[[#This Row],[Horas Iniciales]]/4)</f>
+        <v>6.75</v>
+      </c>
+      <c r="V55">
+        <f>Tabla612[[#This Row],[Semana 3]]-(Tabla612[[#This Row],[Horas Iniciales]]/4)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="56" spans="1:16" ht="15">
+    <row r="56" spans="1:22" ht="15">
       <c r="A56" s="50"/>
       <c r="B56" s="81"/>
       <c r="C56" s="17"/>
@@ -10436,80 +10674,10 @@
       <c r="F56" s="54"/>
       <c r="G56" s="81"/>
       <c r="H56" s="71">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I56" s="57"/>
-    </row>
-    <row r="63" spans="1:16">
-      <c r="A63" t="s">
-        <v>50</v>
-      </c>
-      <c r="B63" t="s">
-        <v>45</v>
-      </c>
-      <c r="C63" t="s">
-        <v>47</v>
-      </c>
-      <c r="D63" t="s">
-        <v>46</v>
-      </c>
-      <c r="E63" t="s">
-        <v>48</v>
-      </c>
-      <c r="F63" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="64" spans="1:16">
-      <c r="A64" t="s">
-        <v>51</v>
-      </c>
-      <c r="B64">
-        <f>L49+L38+L27+L15+L4</f>
-        <v>27</v>
-      </c>
-      <c r="C64">
-        <f>M49+M38+M27+M15+M4</f>
-        <v>20.5</v>
-      </c>
-      <c r="D64">
-        <f>N49+N38+N27+N15+N4</f>
-        <v>20.5</v>
-      </c>
-      <c r="E64">
-        <f>O49+O38+O27+O15+O4</f>
-        <v>20.5</v>
-      </c>
-      <c r="F64">
-        <f>P49+P38+P27+P15+P4</f>
-        <v>20.5</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6">
-      <c r="A65" t="s">
-        <v>52</v>
-      </c>
-      <c r="B65">
-        <f>B64</f>
-        <v>27</v>
-      </c>
-      <c r="C65">
-        <f>Tabla612[[#This Row],[Horas Iniciales]]-(Tabla612[[#This Row],[Horas Iniciales]]/4)</f>
-        <v>20.25</v>
-      </c>
-      <c r="D65">
-        <f>Tabla612[[#This Row],[Semana 1]]-(Tabla612[[#This Row],[Horas Iniciales]]/4)</f>
-        <v>13.5</v>
-      </c>
-      <c r="E65">
-        <f>Tabla612[[#This Row],[Semana 2]]-(Tabla612[[#This Row],[Horas Iniciales]]/4)</f>
-        <v>6.75</v>
-      </c>
-      <c r="F65">
-        <f>Tabla612[[#This Row],[Semana 3]]-(Tabla612[[#This Row],[Horas Iniciales]]/4)</f>
-        <v>0</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0.39370078740157477" bottom="0.39370078740157477" header="0" footer="0"/>

</xml_diff>

<commit_message>
Actualizadas las horas de trabajo
</commit_message>
<xml_diff>
--- a/Documentos/Sprints.xlsx
+++ b/Documentos/Sprints.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\parra\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\FCUD\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="70">
   <si>
     <t>Nombre</t>
   </si>
@@ -242,6 +242,9 @@
   <si>
     <t>Se decidieron los objetivos para la siguiente semana, se mostró el progreso semanal, y se avanzó en el esqueleto HTML</t>
   </si>
+  <si>
+    <t>Sábado y Domingo</t>
+  </si>
 </sst>
 </file>
 
@@ -251,7 +254,7 @@
     <numFmt numFmtId="164" formatCode="dddd\ dd&quot; de &quot;mmmm&quot; de &quot;yyyy"/>
     <numFmt numFmtId="165" formatCode="hh\:mm\ AM/PM"/>
   </numFmts>
-  <fonts count="31">
+  <fonts count="30">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -362,13 +365,6 @@
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
       <charset val="1"/>
     </font>
     <font>
@@ -990,8 +986,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyBorder="0" applyProtection="0"/>
@@ -1002,10 +998,10 @@
     <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="19" borderId="2" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="19" borderId="2" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1054,11 +1050,11 @@
     <xf numFmtId="0" fontId="11" fillId="12" borderId="20" xfId="18" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="19" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="16" borderId="22" xfId="23" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="2" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="2" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="12" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="12" xfId="21" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="14" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="2" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="2" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="12" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="12" xfId="21" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="14" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="16" borderId="23" xfId="23" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="11" fillId="12" borderId="12" xfId="18" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="14" fillId="13" borderId="24" xfId="20" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -1068,38 +1064,38 @@
     <xf numFmtId="0" fontId="15" fillId="15" borderId="22" xfId="22" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="12" fillId="10" borderId="12" xfId="16" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="12" fillId="10" borderId="1" xfId="16" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="22" xfId="23" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="22" xfId="23" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="12" fillId="14" borderId="12" xfId="21" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="25" xfId="11" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="22" fillId="21" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="22" fillId="22" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="21" fillId="21" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="21" fillId="22" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="11" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="3" xfId="24" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="3" xfId="24" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="3" xfId="24" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="3" xfId="24" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="17" borderId="3" xfId="25" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="3" xfId="25" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="13" borderId="2" xfId="20" applyFont="1" applyAlignment="1" applyProtection="1">
@@ -1109,17 +1105,16 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="6" applyFont="1"/>
-    <xf numFmtId="0" fontId="24" fillId="17" borderId="20" xfId="25" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="20" xfId="25" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="14" fillId="13" borderId="2" xfId="20" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="11" fillId="18" borderId="20" xfId="26" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="9" fillId="27" borderId="20" xfId="11" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="6"/>
-    <xf numFmtId="0" fontId="24" fillId="17" borderId="1" xfId="25" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="1" xfId="25" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="11" fillId="18" borderId="1" xfId="26" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="25" fillId="19" borderId="2" xfId="27" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="25" fillId="27" borderId="2" xfId="27" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="1" xfId="11" applyFont="1"/>
-    <xf numFmtId="0" fontId="26" fillId="6" borderId="0" xfId="6" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="19" borderId="2" xfId="27" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="2" xfId="27" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="25" fillId="6" borderId="0" xfId="6" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="11"/>
     <xf numFmtId="0" fontId="14" fillId="13" borderId="2" xfId="20" applyProtection="1"/>
     <xf numFmtId="0" fontId="15" fillId="15" borderId="22" xfId="22" applyBorder="1" applyProtection="1"/>
@@ -1128,12 +1123,13 @@
     <xf numFmtId="0" fontId="14" fillId="13" borderId="2" xfId="20"/>
     <xf numFmtId="0" fontId="16" fillId="16" borderId="2" xfId="23" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="11" borderId="2" xfId="17" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="30" fillId="8" borderId="21" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="8" borderId="21" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="12" borderId="5" xfId="18" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="29" fillId="8" borderId="1" xfId="11" applyFont="1"/>
   </cellXfs>
   <cellStyles count="28">
     <cellStyle name="Accent 1 5" xfId="1"/>
@@ -1400,13 +1396,13 @@
                   <c:v>1.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.25</c:v>
+                  <c:v>-2.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.25</c:v>
+                  <c:v>-2.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.25</c:v>
+                  <c:v>-2.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3208,13 +3204,13 @@
                   <c:v>3.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.5</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.5</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.5</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3654,13 +3650,13 @@
                   <c:v>12.15</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.9499999999999993</c:v>
+                  <c:v>2.4499999999999993</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.9499999999999993</c:v>
+                  <c:v>2.4499999999999993</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.9499999999999993</c:v>
+                  <c:v>2.4499999999999993</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4733,7 +4729,7 @@
   <dimension ref="A1:V58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -4780,7 +4776,7 @@
       <c r="F3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="105" t="s">
+      <c r="G3" s="104" t="s">
         <v>6</v>
       </c>
       <c r="H3" s="4" t="s">
@@ -4829,7 +4825,7 @@
         <f t="shared" ref="H4:H11" si="0">D4+E4+F4+G4</f>
         <v>1.25</v>
       </c>
-      <c r="I4" s="97" t="s">
+      <c r="I4" s="96" t="s">
         <v>17</v>
       </c>
       <c r="Q4" t="s">
@@ -4846,15 +4842,15 @@
       </c>
       <c r="T4">
         <f>S4-E6-E7</f>
-        <v>1.25</v>
+        <v>-2.25</v>
       </c>
       <c r="U4">
         <f>T4-F8-F9</f>
-        <v>1.25</v>
+        <v>-2.25</v>
       </c>
       <c r="V4">
         <f>U4-G10-G11</f>
-        <v>1.25</v>
+        <v>-2.25</v>
       </c>
     </row>
     <row r="5" spans="1:22" ht="15">
@@ -4876,7 +4872,7 @@
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="I5" s="99"/>
+      <c r="I5" s="98"/>
       <c r="Q5" t="s">
         <v>20</v>
       </c>
@@ -4910,13 +4906,13 @@
       <c r="D6" s="21"/>
       <c r="E6" s="20">
         <f>Antonio!G5</f>
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="F6" s="21"/>
       <c r="G6" s="21"/>
       <c r="H6" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="I6" s="22"/>
     </row>
@@ -4980,7 +4976,7 @@
         <v>0</v>
       </c>
       <c r="I10" s="19"/>
-      <c r="J10" s="102"/>
+      <c r="J10" s="101"/>
     </row>
     <row r="11" spans="1:22" ht="15">
       <c r="A11" s="27"/>
@@ -5021,7 +5017,7 @@
       <c r="H14" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="I14" s="104" t="s">
+      <c r="I14" s="103" t="s">
         <v>8</v>
       </c>
       <c r="Q14" s="2" t="s">
@@ -5064,7 +5060,7 @@
         <f t="shared" ref="H15:H23" si="1">D15+E15+F15+G15</f>
         <v>0.5</v>
       </c>
-      <c r="I15" s="101" t="s">
+      <c r="I15" s="100" t="s">
         <v>66</v>
       </c>
       <c r="Q15" t="s">
@@ -5111,7 +5107,7 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="I16" s="95"/>
+      <c r="I16" s="94"/>
       <c r="Q16" t="s">
         <v>20</v>
       </c>
@@ -5155,7 +5151,7 @@
         <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
-      <c r="I17" s="96" t="s">
+      <c r="I17" s="95" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5176,7 +5172,7 @@
         <f t="shared" si="1"/>
         <v>1.6</v>
       </c>
-      <c r="I18" s="100"/>
+      <c r="I18" s="99"/>
     </row>
     <row r="19" spans="1:22" ht="15">
       <c r="A19" s="40"/>
@@ -5368,7 +5364,7 @@
         <f t="shared" si="2"/>
         <v>2.1</v>
       </c>
-      <c r="I28" s="95"/>
+      <c r="I28" s="94"/>
       <c r="Q28" t="s">
         <v>20</v>
       </c>
@@ -5410,7 +5406,7 @@
         <f t="shared" si="2"/>
         <v>1.6</v>
       </c>
-      <c r="I29" s="98" t="s">
+      <c r="I29" s="97" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5557,7 +5553,7 @@
         <f t="shared" ref="H38:H44" si="3">D38+E38+F38+G38</f>
         <v>1.5</v>
       </c>
-      <c r="I38" s="96" t="s">
+      <c r="I38" s="95" t="s">
         <v>17</v>
       </c>
       <c r="Q38" t="s">
@@ -5604,7 +5600,7 @@
         <f t="shared" si="3"/>
         <v>1.5</v>
       </c>
-      <c r="I39" s="95"/>
+      <c r="I39" s="94"/>
       <c r="Q39" t="s">
         <v>20</v>
       </c>
@@ -5754,7 +5750,7 @@
         <f t="shared" ref="H48:H55" si="4">D48+E48+F48+G48</f>
         <v>1.75</v>
       </c>
-      <c r="I48" s="96" t="s">
+      <c r="I48" s="95" t="s">
         <v>17</v>
       </c>
       <c r="Q48" s="2" t="s">
@@ -5795,7 +5791,7 @@
         <f t="shared" si="4"/>
         <v>1.25</v>
       </c>
-      <c r="I49" s="95"/>
+      <c r="I49" s="94"/>
       <c r="Q49" t="s">
         <v>18</v>
       </c>
@@ -5810,15 +5806,15 @@
       </c>
       <c r="T49">
         <f>S49-E50-E51</f>
-        <v>3.5</v>
+        <v>0.5</v>
       </c>
       <c r="U49">
         <f>T49-F52-F53</f>
-        <v>3.5</v>
+        <v>0.5</v>
       </c>
       <c r="V49">
         <f>U49-G54-G55</f>
-        <v>3.5</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="50" spans="1:22" ht="15">
@@ -5830,13 +5826,13 @@
       <c r="D50" s="21"/>
       <c r="E50" s="20">
         <f>Fernando!G5</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F50" s="21"/>
       <c r="G50" s="21"/>
       <c r="H50" s="18">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I50" s="47"/>
       <c r="Q50" t="s">
@@ -5954,15 +5950,15 @@
       </c>
       <c r="T54">
         <f>T49+T38+T27+T15+T4</f>
-        <v>8.9499999999999993</v>
+        <v>2.4499999999999993</v>
       </c>
       <c r="U54">
         <f>U49+U38+U27+U15+U4</f>
-        <v>8.9499999999999993</v>
+        <v>2.4499999999999993</v>
       </c>
       <c r="V54">
         <f>V49+V38+V27+V15+V4</f>
-        <v>8.9499999999999993</v>
+        <v>2.4499999999999993</v>
       </c>
     </row>
     <row r="55" spans="1:22" ht="15">
@@ -6033,8 +6029,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -6123,7 +6119,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="71.25">
+    <row r="8" spans="1:3" ht="42.75">
       <c r="A8" s="67" t="s">
         <v>45</v>
       </c>
@@ -6157,7 +6153,7 @@
       <c r="B12" s="60">
         <v>43738</v>
       </c>
-      <c r="C12" s="103"/>
+      <c r="C12" s="102"/>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="72" t="s">
@@ -6182,7 +6178,7 @@
       <c r="B15" s="64" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="102"/>
+      <c r="C15" s="101"/>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="74" t="s">
@@ -6395,10 +6391,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H6"/>
+  <dimension ref="A2:H13"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:B6"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -6491,27 +6487,35 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="15">
-      <c r="A5" s="94" t="s">
+      <c r="A5" s="93" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="94" t="s">
+      <c r="B5" s="93" t="s">
         <v>65</v>
       </c>
       <c r="C5" s="83">
         <v>2</v>
       </c>
-      <c r="D5" s="84"/>
-      <c r="E5" s="85"/>
-      <c r="F5" s="94"/>
+      <c r="D5" s="84">
+        <v>2</v>
+      </c>
+      <c r="E5" s="85">
+        <v>1.5</v>
+      </c>
+      <c r="F5" s="93" t="s">
+        <v>69</v>
+      </c>
       <c r="G5" s="87">
         <f>Tabla248918[[#This Row],[Horas Trabajadas en Reunion]]+Tabla248918[[#This Row],[Horas Autónomas]]</f>
-        <v>0</v>
-      </c>
-      <c r="H5" s="94"/>
+        <v>3.5</v>
+      </c>
+      <c r="H5" s="93" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="6" spans="1:8" ht="15">
-      <c r="A6" s="94"/>
-      <c r="B6" s="94" t="s">
+      <c r="A6" s="93"/>
+      <c r="B6" s="93" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="88">
@@ -6519,12 +6523,18 @@
       </c>
       <c r="D6" s="84"/>
       <c r="E6" s="89"/>
-      <c r="F6" s="94"/>
+      <c r="F6" s="93"/>
       <c r="G6" s="87">
         <f>Tabla248918[[#This Row],[Horas Trabajadas en Reunion]]+Tabla248918[[#This Row],[Horas Autónomas]]</f>
         <v>0</v>
       </c>
-      <c r="H6" s="94"/>
+      <c r="H6" s="93"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="F10" s="101"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="F13" s="101"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -6540,7 +6550,7 @@
   <dimension ref="A2:H10"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -6656,10 +6666,10 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="15">
-      <c r="A6" s="94" t="s">
+      <c r="A6" s="93" t="s">
         <v>64</v>
       </c>
-      <c r="B6" s="94" t="s">
+      <c r="B6" s="93" t="s">
         <v>25</v>
       </c>
       <c r="C6" s="83">
@@ -6676,13 +6686,13 @@
         <f>Tabla24[[#This Row],[Horas Trabajadas en Reunion]]+Tabla24[[#This Row],[Horas Autónomas]]</f>
         <v>1.6</v>
       </c>
-      <c r="H6" s="94" t="s">
+      <c r="H6" s="93" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15">
-      <c r="A7" s="94"/>
-      <c r="B7" s="94" t="s">
+      <c r="A7" s="93"/>
+      <c r="B7" s="93" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="88">
@@ -6690,12 +6700,12 @@
       </c>
       <c r="D7" s="84"/>
       <c r="E7" s="89"/>
-      <c r="F7" s="94"/>
+      <c r="F7" s="93"/>
       <c r="G7" s="87">
         <f>Tabla24[[#This Row],[Horas Trabajadas en Reunion]]+Tabla24[[#This Row],[Horas Autónomas]]</f>
         <v>0</v>
       </c>
-      <c r="H7" s="94"/>
+      <c r="H7" s="93"/>
     </row>
     <row r="10" spans="1:8">
       <c r="H10" s="1"/>
@@ -6804,10 +6814,10 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="15">
-      <c r="A5" s="94" t="s">
+      <c r="A5" s="93" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="94" t="s">
+      <c r="B5" s="93" t="s">
         <v>25</v>
       </c>
       <c r="C5" s="83">
@@ -6824,13 +6834,13 @@
         <f>Tabla248[[#This Row],[Horas Trabajadas en Reunion]]+Tabla248[[#This Row],[Horas Autónomas]]</f>
         <v>1.6</v>
       </c>
-      <c r="H5" s="94" t="s">
+      <c r="H5" s="93" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15">
-      <c r="A6" s="94"/>
-      <c r="B6" s="94" t="s">
+      <c r="A6" s="93"/>
+      <c r="B6" s="93" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="88">
@@ -6838,12 +6848,12 @@
       </c>
       <c r="D6" s="84"/>
       <c r="E6" s="89"/>
-      <c r="F6" s="94"/>
+      <c r="F6" s="93"/>
       <c r="G6" s="87">
         <f>Tabla248[[#This Row],[Horas Trabajadas en Reunion]]+Tabla248[[#This Row],[Horas Autónomas]]</f>
         <v>0</v>
       </c>
-      <c r="H6" s="94"/>
+      <c r="H6" s="93"/>
     </row>
     <row r="8" spans="1:8">
       <c r="G8" s="1"/>
@@ -6859,10 +6869,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H7"/>
+  <dimension ref="A2:H10"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -6872,7 +6882,7 @@
     <col min="3" max="3" width="12.5" customWidth="1"/>
     <col min="4" max="4" width="12.75" customWidth="1"/>
     <col min="5" max="5" width="12.375" customWidth="1"/>
-    <col min="6" max="6" width="12.5" customWidth="1"/>
+    <col min="6" max="6" width="15.625" customWidth="1"/>
     <col min="7" max="7" width="13.625" customWidth="1"/>
     <col min="8" max="8" width="19.5" customWidth="1"/>
     <col min="9" max="1025" width="10.625" customWidth="1"/>
@@ -6945,10 +6955,10 @@
       <c r="E4" s="89">
         <v>1.5</v>
       </c>
-      <c r="F4" s="92" t="s">
+      <c r="F4" s="105" t="s">
         <v>61</v>
       </c>
-      <c r="G4" s="93">
+      <c r="G4" s="92">
         <f>Tabla2489[[#This Row],[Horas Trabajadas en Reunion]]+E4</f>
         <v>1.5</v>
       </c>
@@ -6957,10 +6967,10 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="15">
-      <c r="A5" s="94" t="s">
+      <c r="A5" s="93" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="94" t="s">
+      <c r="B5" s="93" t="s">
         <v>30</v>
       </c>
       <c r="C5" s="88">
@@ -6968,15 +6978,18 @@
       </c>
       <c r="D5" s="84"/>
       <c r="E5" s="89"/>
-      <c r="F5" s="94"/>
-      <c r="G5" s="93">
+      <c r="F5" s="93"/>
+      <c r="G5" s="92">
         <f>Tabla2489[[#This Row],[Horas Trabajadas en Reunion]]+Tabla2489[[#This Row],[Horas Autónomas]]</f>
         <v>0</v>
       </c>
-      <c r="H5" s="94"/>
+      <c r="H5" s="93"/>
     </row>
     <row r="7" spans="1:8">
       <c r="F7" s="1"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="D10" s="101"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -6989,10 +7002,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H6"/>
+  <dimension ref="A2:H11"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -7004,7 +7017,8 @@
     <col min="5" max="5" width="12.375" customWidth="1"/>
     <col min="6" max="6" width="17.75" customWidth="1"/>
     <col min="7" max="7" width="13.625" customWidth="1"/>
-    <col min="8" max="1025" width="10.625" customWidth="1"/>
+    <col min="8" max="8" width="24.625" customWidth="1"/>
+    <col min="9" max="1025" width="10.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:8" ht="48" customHeight="1">
@@ -7086,27 +7100,35 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="15">
-      <c r="A5" s="94" t="s">
+      <c r="A5" s="93" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="94" t="s">
+      <c r="B5" s="93" t="s">
         <v>65</v>
       </c>
       <c r="C5" s="83">
         <v>2</v>
       </c>
-      <c r="D5" s="84"/>
-      <c r="E5" s="85"/>
-      <c r="F5" s="94"/>
+      <c r="D5" s="84">
+        <v>2</v>
+      </c>
+      <c r="E5" s="85">
+        <v>1</v>
+      </c>
+      <c r="F5" s="93" t="s">
+        <v>62</v>
+      </c>
       <c r="G5" s="87">
         <f>Tabla248910[[#This Row],[Horas Autónomas]]+Tabla248910[[#This Row],[Horas Trabajadas en Reunion]]</f>
-        <v>0</v>
-      </c>
-      <c r="H5" s="94"/>
+        <v>3</v>
+      </c>
+      <c r="H5" s="93" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="6" spans="1:8" ht="15">
-      <c r="A6" s="94"/>
-      <c r="B6" s="94" t="s">
+      <c r="A6" s="93"/>
+      <c r="B6" s="93" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="88">
@@ -7114,18 +7136,25 @@
       </c>
       <c r="D6" s="84"/>
       <c r="E6" s="89"/>
-      <c r="F6" s="94"/>
+      <c r="F6" s="93"/>
       <c r="G6" s="87">
         <f>Tabla248910[[#This Row],[Horas Autónomas]]+Tabla248910[[#This Row],[Horas Trabajadas en Reunion]]</f>
         <v>0</v>
       </c>
-      <c r="H6" s="94"/>
+      <c r="H6" s="93"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="E9" s="101"/>
+      <c r="F9" s="101"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="H11" s="101"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Reunion Semanal con Cuartos Años
</commit_message>
<xml_diff>
--- a/Documentos/Sprints.xlsx
+++ b/Documentos/Sprints.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1 - Grupo" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="91">
   <si>
     <t>Nombre</t>
   </si>
@@ -298,6 +298,15 @@
   </si>
   <si>
     <t>Se discutieron los objetivos a seguir para la otra semana, se trabajará durante la semana</t>
+  </si>
+  <si>
+    <t>Todos menos Maximiliano y Matías</t>
+  </si>
+  <si>
+    <t>Reunión semanal para mostrar progreso y decidir objetivos</t>
+  </si>
+  <si>
+    <t>Se mostro el progreso del HTML y la base de datos MongoDB</t>
   </si>
 </sst>
 </file>
@@ -1789,7 +1798,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1869,7 +1877,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -1993,7 +2000,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -2149,7 +2155,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -2693,7 +2698,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2773,7 +2777,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -2897,7 +2900,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -3053,7 +3055,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -6102,8 +6103,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C53"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -6224,7 +6225,7 @@
         <v>37</v>
       </c>
       <c r="B12" s="60">
-        <v>43738</v>
+        <v>43707</v>
       </c>
       <c r="C12" s="101"/>
     </row>
@@ -6290,7 +6291,7 @@
         <v>37</v>
       </c>
       <c r="B21" s="60">
-        <v>43747</v>
+        <v>43714</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -6348,49 +6349,63 @@
       <c r="A29" s="70" t="s">
         <v>36</v>
       </c>
-      <c r="B29" s="58"/>
+      <c r="B29" s="58">
+        <v>4</v>
+      </c>
       <c r="C29" s="58"/>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="71" t="s">
         <v>37</v>
       </c>
-      <c r="B30" s="60"/>
+      <c r="B30" s="60">
+        <v>43722</v>
+      </c>
       <c r="C30" s="60"/>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="72" t="s">
         <v>38</v>
       </c>
-      <c r="B31" s="62"/>
+      <c r="B31" s="62">
+        <v>0.66666666666666663</v>
+      </c>
       <c r="C31" s="62"/>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="72" t="s">
         <v>39</v>
       </c>
-      <c r="B32" s="62"/>
+      <c r="B32" s="62">
+        <v>0.6875</v>
+      </c>
       <c r="C32" s="62"/>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="73" t="s">
         <v>40</v>
       </c>
-      <c r="B33" s="64"/>
+      <c r="B33" s="64" t="s">
+        <v>88</v>
+      </c>
       <c r="C33" s="64"/>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="74" t="s">
         <v>42</v>
       </c>
-      <c r="B34" s="66"/>
+      <c r="B34" s="66" t="s">
+        <v>89</v>
+      </c>
       <c r="C34" s="66"/>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" ht="28.5">
       <c r="A35" s="75" t="s">
         <v>45</v>
       </c>
-      <c r="B35" s="76"/>
+      <c r="B35" s="76" t="s">
+        <v>90</v>
+      </c>
       <c r="C35" s="76"/>
     </row>
     <row r="37" spans="1:3">
@@ -6531,7 +6546,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>

</xml_diff>